<commit_message>
fix bug in agile capital investment; implement titer/productivity specification
</commit_message>
<xml_diff>
--- a/BioSTEAM 2.x.x/biorefineries/lipidcane2g/lipidcane_spearman_-1_agile.xlsx
+++ b/BioSTEAM 2.x.x/biorefineries/lipidcane2g/lipidcane_spearman_-1_agile.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="54">
   <si>
     <t>Element</t>
   </si>
@@ -70,7 +70,7 @@
     <t>Parameter</t>
   </si>
   <si>
-    <t>Stream-sugarcane</t>
+    <t>biorefinery</t>
   </si>
   <si>
     <t>Stream-ethanol</t>
@@ -82,16 +82,13 @@
     <t>Stream-natural gas</t>
   </si>
   <si>
-    <t>biorefinery</t>
-  </si>
-  <si>
     <t>Stream-crude glycerol</t>
   </si>
   <si>
     <t>Stream-pure glycerine</t>
   </si>
   <si>
-    <t>Stream-cellulase</t>
+    <t>cellulase</t>
   </si>
   <si>
     <t>Pretreatment reactor system</t>
@@ -103,76 +100,82 @@
     <t>Cofermenation</t>
   </si>
   <si>
+    <t>lipidcane</t>
+  </si>
+  <si>
+    <t>lipidsorghum</t>
+  </si>
+  <si>
+    <t>Lipid retention [%]</t>
+  </si>
+  <si>
+    <t>Bagasse lipid extraction efficiency [%]</t>
+  </si>
+  <si>
+    <t>Capacity [ton/hr]</t>
+  </si>
+  <si>
+    <t>Price [USD/gal]</t>
+  </si>
+  <si>
+    <t>Price [USD/cf]</t>
+  </si>
+  <si>
+    <t>Electricity price [USD/kWh]</t>
+  </si>
+  <si>
+    <t>Operating days [day/yr]</t>
+  </si>
+  <si>
+    <t>IRR [%]</t>
+  </si>
+  <si>
+    <t>Price [USD/kg]</t>
+  </si>
+  <si>
+    <t>Cellulase loading [wt. % cellulose]</t>
+  </si>
+  <si>
+    <t>Base cost [million USD]</t>
+  </si>
+  <si>
+    <t>Cane glucose yield [%]</t>
+  </si>
+  <si>
+    <t>Sorghum glucose yield [%]</t>
+  </si>
+  <si>
+    <t>Cane xylose yield [%]</t>
+  </si>
+  <si>
+    <t>Sorghum xylose yield [%]</t>
+  </si>
+  <si>
+    <t>Glucose to ethanol yield [%]</t>
+  </si>
+  <si>
+    <t>Xylose to ethanol yield [%]</t>
+  </si>
+  <si>
+    <t>Cane  PL [% lipid]</t>
+  </si>
+  <si>
+    <t>Sorghum  PL [% lipid]</t>
+  </si>
+  <si>
+    <t>Cane  FFA [% lipid]</t>
+  </si>
+  <si>
+    <t>Sorghum  FFA [% lipid]</t>
+  </si>
+  <si>
     <t>Cane lipid content [dry wt. %]</t>
   </si>
   <si>
     <t>Relative sorghum lipid content [dry wt. %]</t>
   </si>
   <si>
-    <t>Lipid retention [%]</t>
-  </si>
-  <si>
-    <t>Bagasse lipid extraction efficiency [%]</t>
-  </si>
-  <si>
-    <t>Capacity [ton/hr]</t>
-  </si>
-  <si>
-    <t>Cane  PL [% lipid]</t>
-  </si>
-  <si>
-    <t>Sorghum  PL [% lipid]</t>
-  </si>
-  <si>
-    <t>Cane  FFA [% lipid]</t>
-  </si>
-  <si>
-    <t>Sorghum  FFA [% lipid]</t>
-  </si>
-  <si>
     <t>TAG to  FFA conversion [% lipid]</t>
-  </si>
-  <si>
-    <t>Price [USD/gal]</t>
-  </si>
-  <si>
-    <t>Price [USD/cf]</t>
-  </si>
-  <si>
-    <t>Electricity price [USD/kWh]</t>
-  </si>
-  <si>
-    <t>Operating days [day/yr]</t>
-  </si>
-  <si>
-    <t>IRR [%]</t>
-  </si>
-  <si>
-    <t>Price [USD/kg]</t>
-  </si>
-  <si>
-    <t>Cellulase loading [wt. % cellulose]</t>
-  </si>
-  <si>
-    <t>Base cost [million USD]</t>
-  </si>
-  <si>
-    <t>Cane glucose yield [%]</t>
-  </si>
-  <si>
-    <t>Sorghum glucose yield [%]</t>
-  </si>
-  <si>
-    <t>Cane xylose yield [%]</t>
-  </si>
-  <si>
-    <t>Sorghum xylose yield [%]</t>
-  </si>
-  <si>
-    <t>Glucose to ethanol yield [%]</t>
-  </si>
-  <si>
-    <t>Xylose to ethanol yield [%]</t>
   </si>
 </sst>
 </file>
@@ -617,169 +620,177 @@
         <v>18</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C4">
-        <v>-0.04681225081225081</v>
+        <v>-0.004501072501072501</v>
       </c>
       <c r="E4">
-        <v>0.04806985206985207</v>
+        <v>-0.03305246105246105</v>
       </c>
       <c r="F4">
-        <v>-0.03258542058542059</v>
+        <v>-0.01978691578691579</v>
       </c>
       <c r="H4">
-        <v>0.01998414798414799</v>
+        <v>0.02662152262152262</v>
       </c>
       <c r="I4">
-        <v>0.02838746838746839</v>
+        <v>0.02172424572424573</v>
       </c>
       <c r="J4">
-        <v>-0.03999363696199659</v>
+        <v>0.04141639290816179</v>
       </c>
     </row>
     <row r="5" spans="1:16">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C5">
-        <v>-0.01776727776727777</v>
+        <v>-0.001867597867597868</v>
       </c>
       <c r="E5">
-        <v>-0.03238210438210438</v>
+        <v>-0.00825990825990826</v>
       </c>
       <c r="F5">
-        <v>0.004708096708096708</v>
+        <v>-0.03042930642930643</v>
       </c>
       <c r="H5">
-        <v>0.0001624801624801625</v>
+        <v>0.03170943170943171</v>
       </c>
       <c r="I5">
-        <v>-0.00532930132930133</v>
+        <v>0.02876791676791677</v>
       </c>
       <c r="J5">
-        <v>-0.02702230476969367</v>
+        <v>0.01510275174469269</v>
       </c>
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C6">
-        <v>0.0528993168993169</v>
+        <v>0.1346127266127266</v>
       </c>
       <c r="E6">
-        <v>0.02663609063609064</v>
+        <v>-0.04306939906939907</v>
       </c>
       <c r="F6">
-        <v>-0.02711683511683512</v>
+        <v>-0.9661423141423141</v>
       </c>
       <c r="H6">
-        <v>0.02168354168354168</v>
+        <v>1</v>
       </c>
       <c r="I6">
-        <v>0.02813134013134014</v>
+        <v>0.9742967062967064</v>
       </c>
       <c r="J6">
-        <v>0.02122945500545908</v>
+        <v>-0.0354581624241487</v>
       </c>
     </row>
     <row r="7" spans="1:16">
-      <c r="A7" s="1"/>
+      <c r="A7" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="B7" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C7">
-        <v>-0.04047368847368848</v>
+        <v>0.9674192954192956</v>
       </c>
       <c r="E7">
-        <v>0.04562620562620563</v>
+        <v>0.03556708756708757</v>
       </c>
       <c r="F7">
-        <v>0.04658798258798259</v>
+        <v>-0.01645033645033645</v>
       </c>
       <c r="H7">
-        <v>-0.06302514302514303</v>
+        <v>0.008852912852912852</v>
       </c>
       <c r="I7">
-        <v>-0.05220785220785221</v>
+        <v>0.01506395106395106</v>
       </c>
       <c r="J7">
-        <v>-0.04437582155106347</v>
+        <v>-0.02306893812885667</v>
       </c>
     </row>
     <row r="8" spans="1:16">
-      <c r="A8" s="1"/>
+      <c r="A8" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="B8" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C8">
-        <v>0.1196498996498997</v>
+        <v>-0.05016027816027816</v>
       </c>
       <c r="E8">
-        <v>-0.01467600267600268</v>
+        <v>-0.008157116157116158</v>
       </c>
       <c r="F8">
-        <v>-0.9558177198177198</v>
+        <v>-0.01737876537876538</v>
       </c>
       <c r="H8">
-        <v>0.9999999519999522</v>
+        <v>0.02170695370695371</v>
       </c>
       <c r="I8">
-        <v>0.977944025944026</v>
+        <v>0.02235392235392235</v>
       </c>
       <c r="J8">
-        <v>-0.04291538557079922</v>
+        <v>-0.0271477785368859</v>
       </c>
     </row>
     <row r="9" spans="1:16">
-      <c r="A9" s="1"/>
+      <c r="A9" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="B9" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C9">
-        <v>0.00997925797925798</v>
+        <v>-0.01607424407424408</v>
       </c>
       <c r="E9">
-        <v>-0.009481605481605482</v>
+        <v>0.01612180012180012</v>
       </c>
       <c r="F9">
-        <v>-0.02694179094179095</v>
+        <v>0.0187973227973228</v>
       </c>
       <c r="H9">
-        <v>0.03405706605706606</v>
+        <v>-0.02201823401823402</v>
       </c>
       <c r="I9">
-        <v>0.03047064647064647</v>
+        <v>-0.02097303297303297</v>
       </c>
       <c r="J9">
-        <v>0.008478131507756503</v>
+        <v>-0.005378978595608126</v>
       </c>
     </row>
     <row r="10" spans="1:16">
-      <c r="A10" s="1"/>
+      <c r="A10" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="B10" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C10">
-        <v>-0.002148398148398149</v>
+        <v>0.03385072585072586</v>
       </c>
       <c r="E10">
-        <v>-0.07045330645330647</v>
+        <v>0.04347207147207147</v>
       </c>
       <c r="F10">
-        <v>0.09525494325494327</v>
+        <v>-0.01494221094221094</v>
       </c>
       <c r="H10">
-        <v>-0.07773310173310173</v>
+        <v>-0.04006874806874807</v>
       </c>
       <c r="I10">
-        <v>-0.0893987573987574</v>
+        <v>-0.02926784926784927</v>
       </c>
       <c r="J10">
-        <v>0.01557864627939118</v>
+        <v>0.02299174578345476</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -788,22 +799,22 @@
         <v>36</v>
       </c>
       <c r="C11">
-        <v>-0.04208250608250608</v>
+        <v>0.1047741567741568</v>
       </c>
       <c r="E11">
-        <v>-0.02768735168735169</v>
+        <v>0.999997071997072</v>
       </c>
       <c r="F11">
-        <v>0.01659006459006459</v>
+        <v>-0.2032888192888193</v>
       </c>
       <c r="H11">
-        <v>-0.008303348303348303</v>
+        <v>-0.04453936453936454</v>
       </c>
       <c r="I11">
-        <v>-0.01283276483276483</v>
+        <v>0.1744210504210504</v>
       </c>
       <c r="J11">
-        <v>0.03063431181887364</v>
+        <v>-0.0146946166621067</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -812,484 +823,490 @@
         <v>37</v>
       </c>
       <c r="C12">
-        <v>-0.0360972960972961</v>
+        <v>-0.1191535191535192</v>
       </c>
       <c r="E12">
-        <v>0.05713427713427714</v>
+        <v>0.04255212655212656</v>
       </c>
       <c r="F12">
-        <v>0.03212120012120012</v>
+        <v>0.02582227382227383</v>
       </c>
       <c r="H12">
-        <v>-0.05202520002520003</v>
+        <v>-0.03737553737553738</v>
       </c>
       <c r="I12">
-        <v>-0.03755493755493756</v>
+        <v>-0.0290987330987331</v>
       </c>
       <c r="J12">
-        <v>-0.01511407072963495</v>
+        <v>-0.009672423693456592</v>
       </c>
     </row>
     <row r="13" spans="1:16">
-      <c r="A13" s="1"/>
+      <c r="A13" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="B13" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C13">
-        <v>0.01653158853158853</v>
+        <v>0.02678539478539479</v>
       </c>
       <c r="E13">
-        <v>0.01317334917334917</v>
+        <v>-0.01292014892014892</v>
       </c>
       <c r="F13">
-        <v>-0.01983948783948784</v>
+        <v>-0.006443706443706445</v>
       </c>
       <c r="H13">
-        <v>0.01691334491334492</v>
+        <v>0.01010519810519811</v>
       </c>
       <c r="I13">
-        <v>0.01813471813471814</v>
+        <v>0.0061001461001461</v>
       </c>
       <c r="J13">
-        <v>-0.02930390199186858</v>
+        <v>-0.05716696458042957</v>
       </c>
     </row>
     <row r="14" spans="1:16">
       <c r="A14" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C14">
-        <v>0.9727860607860609</v>
+        <v>-0.02881700881700882</v>
       </c>
       <c r="E14">
-        <v>-0.0334987054987055</v>
+        <v>-0.03710524910524911</v>
       </c>
       <c r="F14">
-        <v>-0.0005498045498045497</v>
+        <v>-0.03107118707118707</v>
       </c>
       <c r="H14">
-        <v>0.008541884541884542</v>
+        <v>0.04195118995118996</v>
       </c>
       <c r="I14">
-        <v>0.002840966840966841</v>
+        <v>0.03047980247980248</v>
       </c>
       <c r="J14">
-        <v>-0.002869221765638849</v>
+        <v>-0.01022723804561007</v>
       </c>
     </row>
     <row r="15" spans="1:16">
       <c r="A15" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15">
+        <v>0.03763566163566164</v>
+      </c>
+      <c r="E15">
+        <v>0.04190477390477391</v>
+      </c>
+      <c r="F15">
+        <v>-0.01482115482115482</v>
+      </c>
+      <c r="H15">
+        <v>0.004091860091860092</v>
+      </c>
+      <c r="I15">
+        <v>0.01214672414672415</v>
+      </c>
+      <c r="J15">
+        <v>0.02762860763244512</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C15">
-        <v>-0.01671580071580072</v>
-      </c>
-      <c r="E15">
-        <v>-0.03452320652320653</v>
-      </c>
-      <c r="F15">
-        <v>0.0662937422937423</v>
-      </c>
-      <c r="H15">
-        <v>-0.0581998181998182</v>
-      </c>
-      <c r="I15">
-        <v>-0.06332244332244331</v>
-      </c>
-      <c r="J15">
-        <v>0.01012214724372368</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16">
-      <c r="A16" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="C16">
-        <v>-0.04701887901887902</v>
+        <v>0.009181365181365182</v>
       </c>
       <c r="E16">
-        <v>-0.04332904332904333</v>
+        <v>0.006943938943938945</v>
       </c>
       <c r="F16">
-        <v>0.0128945648945649</v>
+        <v>0.004963144963144963</v>
       </c>
       <c r="H16">
-        <v>0.0008129048129048129</v>
+        <v>-0.00506045306045306</v>
       </c>
       <c r="I16">
-        <v>-0.008551280551280552</v>
+        <v>-0.002931770931770932</v>
       </c>
       <c r="J16">
-        <v>-0.05088534328826314</v>
+        <v>-0.007646576561923753</v>
       </c>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17">
+        <v>3.78960378960379E-05</v>
+      </c>
+      <c r="E17">
+        <v>-0.01577207177207177</v>
+      </c>
+      <c r="F17">
+        <v>0.01341292941292941</v>
+      </c>
+      <c r="H17">
+        <v>-0.003591747591747593</v>
+      </c>
+      <c r="I17">
+        <v>-0.007610803610803612</v>
+      </c>
+      <c r="J17">
+        <v>0.03139679284260154</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C17">
-        <v>0.03777682977682978</v>
-      </c>
-      <c r="E17">
-        <v>-0.0106973626973627</v>
-      </c>
-      <c r="F17">
-        <v>-0.04381876381876382</v>
-      </c>
-      <c r="H17">
-        <v>0.001397125397125397</v>
-      </c>
-      <c r="I17">
-        <v>0.001472761472761473</v>
-      </c>
-      <c r="J17">
-        <v>-0.01051709530453076</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1" t="s">
-        <v>42</v>
-      </c>
       <c r="C18">
-        <v>0.030999750999751</v>
+        <v>0.03557660357660358</v>
       </c>
       <c r="E18">
-        <v>0.999997251997252</v>
+        <v>-0.02747646347646348</v>
       </c>
       <c r="F18">
-        <v>-0.2702212982212983</v>
+        <v>-0.01414575814575815</v>
       </c>
       <c r="H18">
-        <v>-0.01603470403470404</v>
+        <v>0.02656388656388657</v>
       </c>
       <c r="I18">
-        <v>0.1891953571953572</v>
+        <v>0.01905475905475906</v>
       </c>
       <c r="J18">
-        <v>-0.06997621482903184</v>
+        <v>-0.007799549893420844</v>
       </c>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" s="1"/>
       <c r="B19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19">
+        <v>0.0195958515958516</v>
+      </c>
+      <c r="E19">
+        <v>0.007181923181923183</v>
+      </c>
+      <c r="F19">
+        <v>0.02476084876084876</v>
+      </c>
+      <c r="H19">
+        <v>-0.02724641124641125</v>
+      </c>
+      <c r="I19">
+        <v>-0.02550434550434551</v>
+      </c>
+      <c r="J19">
+        <v>-0.01904341106791627</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C19">
-        <v>-0.1222910062910063</v>
-      </c>
-      <c r="E19">
-        <v>-0.02503900903900904</v>
-      </c>
-      <c r="F19">
-        <v>0.01090595890595891</v>
-      </c>
-      <c r="H19">
-        <v>-0.005946389946389947</v>
-      </c>
-      <c r="I19">
-        <v>-0.01142872742872743</v>
-      </c>
-      <c r="J19">
-        <v>-0.01079894372909723</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10">
-      <c r="A20" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="C20">
-        <v>0.0377007257007257</v>
+        <v>-0.08254997854997856</v>
       </c>
       <c r="E20">
-        <v>-0.02534320934320934</v>
+        <v>0.01566698766698767</v>
       </c>
       <c r="F20">
-        <v>-0.006927858927858928</v>
+        <v>0.08136970536970538</v>
       </c>
       <c r="H20">
-        <v>0.01529091929091929</v>
+        <v>-0.08571178971178972</v>
       </c>
       <c r="I20">
-        <v>0.01041791841791842</v>
+        <v>-0.08208890208890209</v>
       </c>
       <c r="J20">
-        <v>-0.03938121408036777</v>
+        <v>0.05587082624518381</v>
       </c>
     </row>
     <row r="21" spans="1:10">
-      <c r="A21" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="A21" s="1"/>
       <c r="B21" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C21">
-        <v>-0.01614551214551214</v>
+        <v>-0.01084174684174684</v>
       </c>
       <c r="E21">
-        <v>0.05035229035229035</v>
+        <v>-0.0404959004959005</v>
       </c>
       <c r="F21">
-        <v>-0.007597087597087598</v>
+        <v>0.02140954540954541</v>
       </c>
       <c r="H21">
-        <v>-0.006391722391722393</v>
+        <v>-0.01738890538890539</v>
       </c>
       <c r="I21">
-        <v>0.003907131907131907</v>
+        <v>-0.02391518391518392</v>
       </c>
       <c r="J21">
-        <v>-0.02024206083568046</v>
+        <v>0.01683896392334662</v>
       </c>
     </row>
     <row r="22" spans="1:10">
       <c r="A22" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C22">
-        <v>-0.04241255441255441</v>
+        <v>0.02481379281379282</v>
       </c>
       <c r="E22">
-        <v>0.01367227367227367</v>
+        <v>-0.04691377091377091</v>
       </c>
       <c r="F22">
-        <v>-0.02205343005343005</v>
+        <v>-0.04128049728049728</v>
       </c>
       <c r="H22">
-        <v>0.02121404121404121</v>
+        <v>0.05203801603801603</v>
       </c>
       <c r="I22">
-        <v>0.02280578280578281</v>
+        <v>0.04107894507894508</v>
       </c>
       <c r="J22">
-        <v>0.01415405080288144</v>
+        <v>-0.009343144558519171</v>
       </c>
     </row>
     <row r="23" spans="1:10">
       <c r="A23" s="1"/>
       <c r="B23" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C23">
-        <v>-0.001542541542541543</v>
+        <v>-0.08555001755001757</v>
       </c>
       <c r="E23">
-        <v>0.02661149061149061</v>
+        <v>0.007395643395643396</v>
       </c>
       <c r="F23">
-        <v>-0.02738942738942739</v>
+        <v>0.002100686100686101</v>
       </c>
       <c r="H23">
-        <v>0.01831504231504232</v>
+        <v>-0.00560934560934561</v>
       </c>
       <c r="I23">
-        <v>0.02353199953199953</v>
+        <v>-0.002294846294846295</v>
       </c>
       <c r="J23">
-        <v>-0.04366620479537292</v>
+        <v>-0.02606150632765931</v>
       </c>
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C24">
-        <v>-0.05971083571083572</v>
+        <v>0.03883125883125883</v>
       </c>
       <c r="E24">
-        <v>-0.0191000111000111</v>
+        <v>0.006403746403746404</v>
       </c>
       <c r="F24">
-        <v>0.05067939867939868</v>
+        <v>0.008064944064944065</v>
       </c>
       <c r="H24">
-        <v>-0.04824052824052825</v>
+        <v>-0.00883923283923284</v>
       </c>
       <c r="I24">
-        <v>-0.05177709977709978</v>
+        <v>-0.009307569307569308</v>
       </c>
       <c r="J24">
-        <v>0.01289424718858361</v>
+        <v>-0.05063637084258524</v>
       </c>
     </row>
     <row r="25" spans="1:10">
       <c r="A25" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C25">
-        <v>-0.01144401544401544</v>
+        <v>0.02257095457095457</v>
       </c>
       <c r="E25">
-        <v>-0.01535139935139935</v>
+        <v>0.03847925047925048</v>
       </c>
       <c r="F25">
-        <v>0.01994861594861595</v>
+        <v>0.02802952002952003</v>
       </c>
       <c r="H25">
-        <v>-0.01335414135414136</v>
+        <v>-0.03985439185439186</v>
       </c>
       <c r="I25">
-        <v>-0.01576635976635977</v>
+        <v>-0.03137812337812338</v>
       </c>
       <c r="J25">
-        <v>0.03086520055917731</v>
+        <v>0.04642575151579705</v>
       </c>
     </row>
     <row r="26" spans="1:10">
-      <c r="A26" s="1"/>
+      <c r="A26" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="B26" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C26">
-        <v>0.0794872514872515</v>
+        <v>-0.03613846813846814</v>
       </c>
       <c r="E26">
-        <v>-0.008639456639456639</v>
+        <v>0.001223797223797224</v>
       </c>
       <c r="F26">
-        <v>0.0006888126888126889</v>
+        <v>0.03543351543351544</v>
       </c>
       <c r="H26">
-        <v>0.002500322500322501</v>
+        <v>-0.03772281772281773</v>
       </c>
       <c r="I26">
-        <v>0.001316821316821317</v>
+        <v>-0.03308152508152509</v>
       </c>
       <c r="J26">
-        <v>-0.01334127776397717</v>
+        <v>0.04834526623658213</v>
       </c>
     </row>
     <row r="27" spans="1:10">
-      <c r="A27" s="1"/>
+      <c r="A27" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="B27" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C27">
-        <v>-0.001854265854265854</v>
+        <v>-0.004066168066168067</v>
       </c>
       <c r="E27">
-        <v>-0.03613506013506013</v>
+        <v>0.02120582120582121</v>
       </c>
       <c r="F27">
-        <v>0.02045398445398446</v>
+        <v>-0.0402980082980083</v>
       </c>
       <c r="H27">
-        <v>-0.01176383976383976</v>
+        <v>0.03296129696129697</v>
       </c>
       <c r="I27">
-        <v>-0.01675240075240075</v>
+        <v>0.03942546342546343</v>
       </c>
       <c r="J27">
-        <v>0.01711779446667805</v>
+        <v>-0.0113573404685411</v>
       </c>
     </row>
     <row r="28" spans="1:10">
-      <c r="A28" s="1"/>
+      <c r="A28" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="B28" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C28">
-        <v>0.003763299763299764</v>
+        <v>0.03222602022602023</v>
       </c>
       <c r="E28">
-        <v>0.01147385947385948</v>
+        <v>0.03546225546225547</v>
       </c>
       <c r="F28">
-        <v>0.02461588861588862</v>
+        <v>-0.004456276456276456</v>
       </c>
       <c r="H28">
-        <v>-0.02956066156066156</v>
+        <v>-0.002368610368610369</v>
       </c>
       <c r="I28">
-        <v>-0.02799691599691599</v>
+        <v>0.003501615501615502</v>
       </c>
       <c r="J28">
-        <v>0.03238084136294953</v>
+        <v>-0.006278032491350406</v>
       </c>
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C29">
-        <v>0.007794823794823795</v>
+        <v>-0.04812610812610813</v>
       </c>
       <c r="E29">
-        <v>-0.03006383406383406</v>
+        <v>0.01038388638388638</v>
       </c>
       <c r="F29">
-        <v>0.007065463065463067</v>
+        <v>0.03042681042681043</v>
       </c>
       <c r="H29">
-        <v>-0.0005543405543405543</v>
+        <v>-0.03702022902022902</v>
       </c>
       <c r="I29">
-        <v>-0.00714010314010314</v>
+        <v>-0.0318975798975799</v>
       </c>
       <c r="J29">
-        <v>0.03466845503423854</v>
+        <v>-0.04143539520963627</v>
       </c>
     </row>
     <row r="30" spans="1:10">
-      <c r="A30" s="1"/>
+      <c r="A30" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="B30" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C30">
-        <v>-0.006987210987210989</v>
+        <v>0.03245832845832846</v>
       </c>
       <c r="E30">
-        <v>0.007657975657975658</v>
+        <v>-0.01014025014025014</v>
       </c>
       <c r="F30">
-        <v>-0.02703381903381903</v>
+        <v>-0.01204323604323604</v>
       </c>
       <c r="H30">
-        <v>0.02383625983625984</v>
+        <v>0.01403754203754204</v>
       </c>
       <c r="I30">
-        <v>0.02638017838017838</v>
+        <v>0.01301083301083301</v>
       </c>
       <c r="J30">
-        <v>-0.01452329385504836</v>
+        <v>-0.02982687482498655</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="C1:P1"/>
-    <mergeCell ref="A4:A13"/>
-    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A18:A21"/>
     <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A25:A28"/>
-    <mergeCell ref="A29:A30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>